<commit_message>
Initial exploration and analysis of university organizations data
Co-authored-by: ambicuity <44251619+ambicuity@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/University_Organizations_Summary.xlsx
+++ b/University_Organizations_Summary.xlsx
@@ -437,7 +437,7 @@
     <col width="50" customWidth="1" min="2" max="2"/>
     <col width="21" customWidth="1" min="3" max="3"/>
     <col width="16" customWidth="1" min="4" max="4"/>
-    <col width="19" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -485,17 +485,17 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" t="n">
         <v>4</v>
       </c>
       <c r="E2" t="n">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Complete</t>
+          <t>Issues</t>
         </is>
       </c>
     </row>
@@ -511,17 +511,17 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D3" t="n">
         <v>80</v>
       </c>
       <c r="E3" t="n">
-        <v>32.5</v>
+        <v>25</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Complete</t>
+          <t>Issues</t>
         </is>
       </c>
     </row>
@@ -537,17 +537,17 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
         <v>5</v>
       </c>
       <c r="E4" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Complete</t>
+          <t>Issues</t>
         </is>
       </c>
     </row>
@@ -563,17 +563,17 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="D5" t="n">
         <v>19</v>
       </c>
       <c r="E5" t="n">
-        <v>447.3684210526316</v>
+        <v>363.1578947368421</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Complete</t>
+          <t>Issues</t>
         </is>
       </c>
     </row>
@@ -589,17 +589,17 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D6" t="n">
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>407.1428571428571</v>
+        <v>342.8571428571428</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Complete</t>
+          <t>Issues</t>
         </is>
       </c>
     </row>
@@ -615,17 +615,17 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
         <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>100</v>
+        <v>66.66666666666666</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Complete</t>
+          <t>Issues</t>
         </is>
       </c>
     </row>
@@ -641,17 +641,17 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="D8" t="n">
         <v>16</v>
       </c>
       <c r="E8" t="n">
-        <v>312.5</v>
+        <v>193.75</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Complete</t>
+          <t>Issues</t>
         </is>
       </c>
     </row>
@@ -667,17 +667,17 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D9" t="n">
         <v>75</v>
       </c>
       <c r="E9" t="n">
-        <v>40</v>
+        <v>42.66666666666667</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Complete</t>
+          <t>Issues</t>
         </is>
       </c>
     </row>
@@ -693,17 +693,17 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" t="n">
         <v>10</v>
       </c>
       <c r="E10" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Complete</t>
+          <t>Issues</t>
         </is>
       </c>
     </row>
@@ -719,17 +719,17 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" t="n">
         <v>15</v>
       </c>
       <c r="E11" t="n">
-        <v>100</v>
+        <v>93.33333333333333</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Complete</t>
+          <t>Issues</t>
         </is>
       </c>
     </row>
@@ -755,7 +755,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Complete</t>
+          <t>Issues</t>
         </is>
       </c>
     </row>

</xml_diff>